<commit_message>
add mouse out command
</commit_message>
<xml_diff>
--- a/src/test/resources/mouseOut/mouseOut.xlsx
+++ b/src/test/resources/mouseOut/mouseOut.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projs\auto-test\src\test\resources\mouseOut\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\projs\auto-test\src\test\resources\mouseOut\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66447677-1976-4B90-A8F2-2B76F6C6BCEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0396B54B-BBAE-4C29-B5E4-FCA6C268DA62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-135" yWindow="-135" windowWidth="29070" windowHeight="15750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -456,21 +456,21 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="8.75" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="19.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.58203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="19.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.5" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -493,7 +493,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="4"/>
       <c r="B2" s="2" t="s">
         <v>7</v>
@@ -510,7 +510,7 @@
       </c>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1">
         <v>1</v>
       </c>

</xml_diff>